<commit_message>
remove files, add compliance figure
</commit_message>
<xml_diff>
--- a/conven_control/data/ros_data.xlsx
+++ b/conven_control/data/ros_data.xlsx
@@ -153,7 +153,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N5" activeCellId="0" sqref="N5"/>
+      <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -161,7 +161,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -723,7 +723,7 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>